<commit_message>
Recap into DOCX version
</commit_message>
<xml_diff>
--- a/Data/Data_Assistant.xlsx
+++ b/Data/Data_Assistant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Proton\ERT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D97C57-EC85-4330-9634-EA89D5450650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBBBEBA-A934-4ECF-9F8E-411639FB7C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2970" windowWidth="16905" windowHeight="12000" xr2:uid="{47162153-D28C-4C06-B23B-39F2F87358B2}"/>
+    <workbookView xWindow="9885" yWindow="3330" windowWidth="16905" windowHeight="12000" xr2:uid="{47162153-D28C-4C06-B23B-39F2F87358B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Assistant</t>
   </si>
@@ -82,6 +82,42 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>Zahra</t>
+  </si>
+  <si>
+    <t>Agus</t>
+  </si>
+  <si>
+    <t>Nori</t>
+  </si>
+  <si>
+    <t>Prasetya</t>
+  </si>
+  <si>
+    <t>Abil</t>
+  </si>
+  <si>
+    <t>Dinul</t>
+  </si>
+  <si>
+    <t>Arinal</t>
+  </si>
+  <si>
+    <t>Said</t>
+  </si>
+  <si>
+    <t>Beling</t>
+  </si>
+  <si>
+    <t>Fajar</t>
+  </si>
+  <si>
+    <t>Ardi</t>
+  </si>
+  <si>
+    <t>Ade</t>
   </si>
 </sst>
 </file>
@@ -433,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C23A84A-5B40-4488-B363-7C567B359C60}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,6 +569,86 @@
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>